<commit_message>
Updates to configuration bundles
</commit_message>
<xml_diff>
--- a/Documentation/DecToHex_Conversion_Table.xlsx
+++ b/Documentation/DecToHex_Conversion_Table.xlsx
@@ -349,38 +349,38 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>248842</v>
+        <v>97389</v>
       </c>
       <c r="C1" t="str">
         <f>DEC2HEX($B1,8)</f>
-        <v>0003CC0A</v>
+        <v>00017C6D</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>96655</v>
+        <v>249524</v>
       </c>
       <c r="C2" t="str">
         <f>DEC2HEX($B2,8)</f>
-        <v>0001798F</v>
+        <v>0003CEB4</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>96070</v>
+        <v>97436</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C6" si="0">DEC2HEX($B3,8)</f>
-        <v>00017746</v>
+        <v>00017C9C</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>248259</v>
+        <v>249593</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>0003C9C3</v>
+        <v>0003CEF9</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>